<commit_message>
Add Project to main branch
</commit_message>
<xml_diff>
--- a/Files_Test/InvalidDataSheet.xlsx
+++ b/Files_Test/InvalidDataSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\New Project\Pulk_Pending_Account\Files_Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F72A01B8-4CCF-48D6-B469-B9596E61D9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F80D8D-B90B-4CE2-A22F-C90D81F695EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3C0DBD8C-DC7F-4369-9E91-824A1AF69384}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>full name</t>
   </si>
@@ -45,9 +45,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
     <t xml:space="preserve">Male </t>
   </si>
   <si>
@@ -93,14 +90,59 @@
     <t xml:space="preserve">NO </t>
   </si>
   <si>
-    <t xml:space="preserve">lol </t>
+    <t xml:space="preserve">515*/**/*-/*/*/* </t>
+  </si>
+  <si>
+    <t>0101001005</t>
+  </si>
+  <si>
+    <t>0101001006</t>
+  </si>
+  <si>
+    <t>0101001007</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0101001001</t>
+  </si>
+  <si>
+    <t>+20101001003</t>
+  </si>
+  <si>
+    <t>e0101001004</t>
+  </si>
+  <si>
+    <t>sdf sjdfb jdhfs dfsn isdfhs isf  juseif lis fsi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">national-id </t>
+  </si>
+  <si>
+    <t>wedwhehhwhd</t>
+  </si>
+  <si>
+    <t>302022022548</t>
+  </si>
+  <si>
+    <t>30256655485265</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c                                </t>
+  </si>
+  <si>
+    <t>30256455485265</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 30256655485265</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0101001002 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +158,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -125,7 +173,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -148,15 +196,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -472,20 +533,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178E2FEC-6C58-43FE-AEAE-F621C17B8359}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" customWidth="1"/>
+    <col min="4" max="4" width="24" style="3" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,10 +563,13 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -512,14 +577,17 @@
       <c r="C2">
         <v>20</v>
       </c>
-      <c r="D2">
-        <v>101001001</v>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5454</v>
       </c>
@@ -529,84 +597,106 @@
       <c r="C3">
         <v>554</v>
       </c>
-      <c r="D3">
-        <v>101001002</v>
+      <c r="D3" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
+      <c r="F4" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="D4">
-        <v>101001003</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F5" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
         <v>20</v>
       </c>
+      <c r="F6" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>101001004</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="D6">
-        <v>101001005</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>101001006</v>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
       </c>
+      <c r="F7" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8">
-        <v>101001007</v>
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" xr:uid="{F2DF64F2-936E-4636-A92E-7D5687DE0DCF}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Add Verification data and runners
</commit_message>
<xml_diff>
--- a/Files_Test/InvalidDataSheet.xlsx
+++ b/Files_Test/InvalidDataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\New Project\Pulk_Pending_Account\Files_Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F80D8D-B90B-4CE2-A22F-C90D81F695EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CD6D34-BB0E-4AC1-BC85-2719A6BCED6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3C0DBD8C-DC7F-4369-9E91-824A1AF69384}"/>
+    <workbookView xWindow="6555" yWindow="2985" windowWidth="21600" windowHeight="9285" xr2:uid="{3C0DBD8C-DC7F-4369-9E91-824A1AF69384}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,15 +96,9 @@
     <t>0101001005</t>
   </si>
   <si>
-    <t>0101001006</t>
-  </si>
-  <si>
     <t>0101001007</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0101001001</t>
-  </si>
-  <si>
     <t>+20101001003</t>
   </si>
   <si>
@@ -135,7 +129,13 @@
     <t xml:space="preserve"> 30256655485265</t>
   </si>
   <si>
-    <t xml:space="preserve">0101001002 </t>
+    <t xml:space="preserve"> 0101001001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0101001002   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0101001006   </t>
   </si>
 </sst>
 </file>
@@ -217,7 +217,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -536,7 +536,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +564,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -578,13 +578,13 @@
         <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -598,13 +598,13 @@
         <v>554</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -618,13 +618,13 @@
         <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -635,13 +635,13 @@
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -658,24 +658,24 @@
         <v>20</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -686,13 +686,13 @@
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
         <v>21</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>